<commit_message>
model tournament input update
</commit_message>
<xml_diff>
--- a/experiment_data/model_tournament/model_tournament_input.xlsx
+++ b/experiment_data/model_tournament/model_tournament_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miche\OneDrive\Desktop\Codenames Progetto PDE\Codenames-LLM\experiment_data\model_tournament\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFD9123-FD44-458A-BF1C-4D7F64BFB9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B735A180-13F8-47B3-904B-393FFB6B1F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="23232" windowHeight="25296" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4608" yWindow="4608" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="19">
   <si>
     <t>red_model</t>
   </si>
@@ -73,16 +73,10 @@
     <t>claude-3-5-haiku-latest</t>
   </si>
   <si>
-    <t>gemini-1.5-flash-latest</t>
-  </si>
-  <si>
-    <t>gemini-1.5-pro-latest</t>
-  </si>
-  <si>
-    <t>llama-3.2-11b-vision</t>
-  </si>
-  <si>
-    <t>llama-3.2-90b-vision</t>
+    <t>llama3.2-11b-vision</t>
+  </si>
+  <si>
+    <t>llama3.2-90b-vision</t>
   </si>
 </sst>
 </file>
@@ -445,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J110"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,18 +548,18 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -573,7 +567,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -581,7 +575,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -589,7 +583,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -597,7 +591,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -605,39 +599,39 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -645,7 +639,7 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -653,7 +647,7 @@
         <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -661,63 +655,63 @@
         <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -725,7 +719,7 @@
         <v>14</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -733,639 +727,231 @@
         <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B42" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B43" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B47" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B51" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B52" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B53" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B54" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B55" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B56" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B57" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B58" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B59" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>17</v>
-      </c>
-      <c r="B60" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>17</v>
-      </c>
-      <c r="B61" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>17</v>
-      </c>
-      <c r="B62" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>17</v>
-      </c>
-      <c r="B63" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>17</v>
-      </c>
-      <c r="B64" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>17</v>
-      </c>
-      <c r="B65" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>17</v>
-      </c>
-      <c r="B66" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>18</v>
-      </c>
-      <c r="B67" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>18</v>
-      </c>
-      <c r="B68" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>18</v>
-      </c>
-      <c r="B69" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>18</v>
-      </c>
-      <c r="B70" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>18</v>
-      </c>
-      <c r="B71" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>18</v>
-      </c>
-      <c r="B72" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>18</v>
-      </c>
-      <c r="B73" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>18</v>
-      </c>
-      <c r="B74" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>18</v>
-      </c>
-      <c r="B75" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>19</v>
-      </c>
-      <c r="B76" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>19</v>
-      </c>
-      <c r="B77" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>19</v>
-      </c>
-      <c r="B78" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>19</v>
-      </c>
-      <c r="B79" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>19</v>
-      </c>
-      <c r="B80" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>19</v>
-      </c>
-      <c r="B81" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>19</v>
-      </c>
-      <c r="B82" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>19</v>
-      </c>
-      <c r="B83" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>19</v>
-      </c>
-      <c r="B84" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>20</v>
-      </c>
-      <c r="B85" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>20</v>
-      </c>
-      <c r="B86" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>20</v>
-      </c>
-      <c r="B87" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>20</v>
-      </c>
-      <c r="B88" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>20</v>
-      </c>
-      <c r="B89" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>20</v>
-      </c>
-      <c r="B90" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>20</v>
-      </c>
-      <c r="B91" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>20</v>
-      </c>
-      <c r="B92" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>20</v>
-      </c>
-      <c r="B93" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>19</v>
-      </c>
-      <c r="B94" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>19</v>
-      </c>
-      <c r="B95" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>19</v>
-      </c>
-      <c r="B96" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>19</v>
-      </c>
-      <c r="B97" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>19</v>
-      </c>
-      <c r="B98" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>19</v>
-      </c>
-      <c r="B99" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>19</v>
-      </c>
-      <c r="B100" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>20</v>
-      </c>
-      <c r="B101" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>20</v>
-      </c>
-      <c r="B102" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>20</v>
-      </c>
-      <c r="B103" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>20</v>
-      </c>
-      <c r="B104" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>20</v>
-      </c>
-      <c r="B105" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>20</v>
-      </c>
-      <c r="B106" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>20</v>
-      </c>
-      <c r="B107" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>20</v>
-      </c>
-      <c r="B108" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>20</v>
-      </c>
-      <c r="B109" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>20</v>
-      </c>
-      <c r="B110" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
try except at getting data
</commit_message>
<xml_diff>
--- a/experiment_data/model_tournament/model_tournament_input.xlsx
+++ b/experiment_data/model_tournament/model_tournament_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miche\OneDrive\Desktop\Codenames Progetto PDE\Codenames-LLM\experiment_data\model_tournament\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B735A180-13F8-47B3-904B-393FFB6B1F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA42D64-63AE-49B0-BDA7-121569EB47F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4608" yWindow="4608" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="22">
   <si>
     <t>red_model</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t>llama3.2-90b-vision</t>
+  </si>
+  <si>
+    <t>gemini-1.5-flash-latest</t>
+  </si>
+  <si>
+    <t>gemini-1.5-pro-latest</t>
+  </si>
+  <si>
+    <t>llama-3.2-11b-vision</t>
   </si>
 </sst>
 </file>
@@ -439,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:J93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -954,6 +963,278 @@
         <v>17</v>
       </c>
     </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>11</v>
+      </c>
+      <c r="B62" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>11</v>
+      </c>
+      <c r="B63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>14</v>
+      </c>
+      <c r="B66" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>14</v>
+      </c>
+      <c r="B67" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>15</v>
+      </c>
+      <c r="B68" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>15</v>
+      </c>
+      <c r="B69" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>16</v>
+      </c>
+      <c r="B70" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>16</v>
+      </c>
+      <c r="B71" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>19</v>
+      </c>
+      <c r="B73" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>19</v>
+      </c>
+      <c r="B74" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>19</v>
+      </c>
+      <c r="B75" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>19</v>
+      </c>
+      <c r="B76" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>19</v>
+      </c>
+      <c r="B77" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>19</v>
+      </c>
+      <c r="B78" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>19</v>
+      </c>
+      <c r="B79" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>19</v>
+      </c>
+      <c r="B80" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>20</v>
+      </c>
+      <c r="B81" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>20</v>
+      </c>
+      <c r="B82" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>20</v>
+      </c>
+      <c r="B83" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>20</v>
+      </c>
+      <c r="B84" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>20</v>
+      </c>
+      <c r="B85" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>20</v>
+      </c>
+      <c r="B86" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>20</v>
+      </c>
+      <c r="B87" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>20</v>
+      </c>
+      <c r="B88" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>20</v>
+      </c>
+      <c r="B89" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>21</v>
+      </c>
+      <c r="B90" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>17</v>
+      </c>
+      <c r="B91" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>18</v>
+      </c>
+      <c r="B92" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>18</v>
+      </c>
+      <c r="B93" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
implement dumb (cib) test (while)
</commit_message>
<xml_diff>
--- a/experiment_data/model_tournament/model_tournament_input.xlsx
+++ b/experiment_data/model_tournament/model_tournament_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miche\OneDrive\Desktop\Codenames Progetto PDE\Codenames-LLM\experiment_data\model_tournament\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490CD340-20EB-4F8B-B834-578343C1C788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C724471-B16A-4A29-AA35-8E0F99A7C245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="23">
   <si>
     <t>red_model</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>llama-3.2-11b-vision</t>
+  </si>
+  <si>
+    <t>red_cib</t>
+  </si>
+  <si>
+    <t>blue_cib</t>
   </si>
 </sst>
 </file>
@@ -445,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J91"/>
+  <dimension ref="A1:L91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,7 +470,7 @@
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,8 +501,14 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -504,7 +516,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -512,7 +524,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -520,7 +532,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -528,7 +540,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -536,7 +548,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -544,7 +556,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -552,7 +564,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -560,7 +572,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -568,7 +580,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -576,7 +588,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -584,7 +596,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -592,7 +604,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -600,7 +612,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -608,7 +620,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>12</v>
       </c>

</xml_diff>